<commit_message>
fix conflict basetest and update create service tcs
</commit_message>
<xml_diff>
--- a/src/main/resources/excels/CreateService.xlsx
+++ b/src/main/resources/excels/CreateService.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20361"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\projectIJ\src\main\resources\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A78CF4-2BBC-4BCB-8420-D2626FC4E138}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F7B44BE-D417-45CA-A428-812AFDD16621}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8484" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -54,92 +54,13 @@
     <t>Error message should be shown correctly</t>
   </si>
   <si>
-    <t>1. Login to Dashboard
-2. Go to Create Service page.
-3. Check create successful</t>
-  </si>
-  <si>
-    <t>Create successfull message should be shown</t>
-  </si>
-  <si>
-    <t>Check normal service on SF</t>
-  </si>
-  <si>
-    <t>1. Go to SF
-2. Search and go to search detail page
-3. Check service infor: Service name, Price, Image, Location, Time, Book Now button, Add to cart button, Description</t>
-  </si>
-  <si>
-    <t>Service infor should be show correctly as created</t>
-  </si>
-  <si>
-    <t>Create service belong to 1 collection</t>
-  </si>
-  <si>
-    <t>Check service belong to 1 collection display on SF</t>
-  </si>
-  <si>
-    <t>1. Go to SF
-2. Search and go to search detail page
-3. Check service infor: Service name, Price, Image, Location, Time, Book Now button, Add to cart button, Description, Collection link
-4. Click on Collection link 
-5. Verify new service display in collection page</t>
-  </si>
-  <si>
-    <t>Service infor should be show correctly as created and shown in collection page</t>
-  </si>
-  <si>
-    <t>Service infor should be show correctly as created and shown in all collection page</t>
-  </si>
-  <si>
     <t>Create listing service</t>
-  </si>
-  <si>
-    <t>Check listing service on SF</t>
-  </si>
-  <si>
-    <t>1. Go to SF
-2. Search and go to search detail page
-3. Check service infor: Service name, Price, Image, Location, Time, Book Now button, Add to cart button, Contact now button, Description, Collection link
-4. Click on Collection link 
-5. Verify new service display in collection page</t>
-  </si>
-  <si>
-    <t>Service infor should be show correctly as created and shown in collection page
-Contact Now button should be shown instead of Book now button and Add to cart button.
-Price should be not shown.</t>
-  </si>
-  <si>
-    <t>Create service has SEO infor</t>
-  </si>
-  <si>
-    <t>Check SEO infor of service on SF</t>
-  </si>
-  <si>
-    <t>1. Go to SF 
-2. Search and go to search detail page
-3. Check meta tag</t>
-  </si>
-  <si>
-    <t>meta tag has name="title", content = &lt;SEO title&gt;
-meta tag has name="description", content = &lt;SEO description&gt;
-meta tag has name="keyword", content = &lt;SEO keyword&gt;
-Service detail page should be navigated from SEO url</t>
   </si>
   <si>
     <t>1. Login to Dashboard
 2. Go to Create Service page.
 3. Check error when save with empty empty
 4. Check error when input out of range</t>
-  </si>
-  <si>
-    <t>Create normal service</t>
-  </si>
-  <si>
-    <t>Create service belong to multiple collection</t>
-  </si>
-  <si>
-    <t>Check service belong to multiple collection on SF</t>
   </si>
   <si>
     <t>CS01</t>
@@ -163,32 +84,73 @@
     <t>CS07</t>
   </si>
   <si>
-    <t>CS08</t>
+    <t>Create normal service and verify on SF</t>
   </si>
   <si>
-    <t>CS09</t>
+    <t>Create service belong to 1 collection and check on SF</t>
   </si>
   <si>
-    <t>CS10</t>
+    <t>1. Login to Dashboard &gt;&gt; Create Service page.
+2. Create service successful
+3. Go to SF &gt;&gt; Search and go to search detail page
+4. Check service infor: Service name, Price, Image, Location, Time, Book Now button, Add to cart button, Description, Collection link
+5. Click on Collection link 
+6. Verify new service display in collection page</t>
   </si>
   <si>
-    <t>CS11</t>
+    <t>Create successfull message should be shown.
+Service infor should be show correctly as created and shown in collection page</t>
   </si>
   <si>
-    <t>CS12</t>
+    <t>Create service belong to multiple collection and check on SF</t>
   </si>
   <si>
-    <t>PASS</t>
+    <t>1. Login to Dashboard &gt;&gt; Create Service page.
+2. Create service successful
+3. Go to SF &gt;&gt; Search and go to search detail page
+4. Check service infor: Service name, Price, Image, Location, Time, Book Now button, Add to cart button, Description, All Services link
+5. Click on All Services link 
+6. Verify new service display in all services page</t>
   </si>
   <si>
-    <t>FAIL</t>
+    <t>1. Login to Dashboard &gt;&gt; Create Service page.
+2. Check create successful
+3. Go to SF &gt;&gt; Search and go to search detail page
+4. Check service infor: Service name, Price, Image, Location, Time, Book Now button, Add to cart button, Contact now button, Description, Collection link
+5. Click on Collection link 
+6. Verify new service display in collection page</t>
+  </si>
+  <si>
+    <t>Create successfull message should be shown.
+Service infor should be show correctly as created and shown in collection page 
+Contact Now button should be shown instead of Book now button and Add to cart button. 
+Price should be not shown.</t>
+  </si>
+  <si>
+    <t>Create service has SEO infor and check on SF</t>
+  </si>
+  <si>
+    <t>1. Login to Dashboard &gt;&gt; Create Service page.
+2. Check create successful
+3. Go to SF &gt;&gt; Search and go to search detail page
+4. Check meta tag</t>
+  </si>
+  <si>
+    <t>Create successfull message should be shown.
+"meta tag has name=""title"", content = &lt;SEO title&gt;
+meta tag has name=""description"", content = &lt;SEO description&gt;
+meta tag has name=""keyword"", content = &lt;SEO keyword&gt;
+Service detail page should be navigated from SEO url"</t>
+  </si>
+  <si>
+    <t>Create successfull message should be shown.
+Service infor should be show correctly as created and shown in all services page</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -495,16 +457,16 @@
   </sheetPr>
   <dimension ref="A1:E1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="11.109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="27.77734375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="38.88671875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="54.109375" collapsed="true"/>
+    <col min="1" max="1" width="11.109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.77734375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="38.88671875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="54.109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -526,7 +488,7 @@
     </row>
     <row r="2" spans="1:5" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>5</v>
@@ -537,196 +499,120 @@
       <c r="D2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="3" spans="1:5" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:5" ht="145.80000000000001" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="145.80000000000001" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="145.80000000000001" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="159" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="79.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="106.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="106.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="119.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" t="s">
-        <v>44</v>
-      </c>
+    </row>
+    <row r="9" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+    </row>
+    <row r="13" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="5"/>
     </row>
     <row r="14" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>

</xml_diff>